<commit_message>
fix bug on message send
</commit_message>
<xml_diff>
--- a/project_management/issues.xlsx
+++ b/project_management/issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Code/LLM/DeepDive/project_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195EEB50-9AA6-CD4B-8B63-71B3ACEA0BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A4A8FC-CA50-974B-8DA5-4678B08007E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="7600" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{0C39C6D7-9AA0-5548-85B5-0775C5B449C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>DeepDive Backlog</t>
   </si>
@@ -162,18 +162,12 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Not Clearing Dialog</t>
-  </si>
-  <si>
     <t>Frontend</t>
   </si>
   <si>
     <t>NewChat</t>
   </si>
   <si>
-    <t>On NewChat the DialogContext is not cleared. The current Chat is not switched to the new chat</t>
-  </si>
-  <si>
     <t>Highlight Active</t>
   </si>
   <si>
@@ -210,10 +204,46 @@
     <t>Backend</t>
   </si>
   <si>
-    <t>Testing needs itown environment</t>
-  </si>
-  <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Switching ContextDialog </t>
+  </si>
+  <si>
+    <t>When a Chat History is deleted the message Dialog should . Should switch to the Next Active Chat. If all chat are deleted the Message Dialog should clear</t>
+  </si>
+  <si>
+    <t>DeleteChat</t>
+  </si>
+  <si>
+    <t>When a new chat is created and there is an active dialog the dialof should switch to the new chat</t>
+  </si>
+  <si>
+    <t>Exact Message Sent Problem</t>
+  </si>
+  <si>
+    <t>ChatPrompt</t>
+  </si>
+  <si>
+    <t>When the same "Exact" message is sent twice the second message is not sent</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Testing needs its own environment</t>
+  </si>
+  <si>
+    <t>sendMessage on dup message</t>
+  </si>
+  <si>
+    <t>If the same message is sent twice the send of the message will not trigger a call to the AI</t>
   </si>
 </sst>
 </file>
@@ -283,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -292,6 +322,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +831,10 @@
     </row>
     <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -808,27 +844,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC055A18-C93F-B143-A6B0-05F466CAD22A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -841,83 +878,146 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
+      <c r="D9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>